<commit_message>
重命名 prompts.py 为 template.py
- 将 prompts.py 重命名为 template.py（更准确反映其作用）
- 更新 send_bulk_emails.py 中的所有导入和引用
- 更新 README.md 中的文档说明
- 更新 .env.example 中的配置说明
- 确保所有引用都已更新，无遗漏
</commit_message>
<xml_diff>
--- a/通用邮件群发/发送列表.xlsx
+++ b/通用邮件群发/发送列表.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,94 +473,32 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>example1@example.com</t>
+          <t>550350664@qq.com</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>变量1示例值</t>
+          <t>Cody</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>变量2示例值</t>
+          <t>哈哈哈</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>变量3示例值</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
+          <t>你好啊</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>宠物.jpg</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>example2@example.com</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>2025-01-20</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>感谢您的支持</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>document.pdf</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>example3@example.com</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>重要</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>测试会议</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>备注信息</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>certificate.jpg</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>receipt.pdf</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>